<commit_message>
correcting linkSD intro appearance bug
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -125,26 +125,26 @@
     <t>DSTATE</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>VOID</t>
   </si>
   <si>
-    <t>0 =Default; Valid Record_x000D_
+    <t>0 =Default; Valid Record
 1 = VOID record</t>
   </si>
   <si>
@@ -221,8 +221,8 @@
     <t>MFILED</t>
   </si>
   <si>
-    <t>0 = Electronic Mode_x000D_
-1 = Paper Mode_x000D_
+    <t>0 = Electronic Mode
+1 = Paper Mode
 2 = Mixed Mode</t>
   </si>
   <si>
@@ -286,7 +286,7 @@
     <t>ALIAS</t>
   </si>
   <si>
-    <t>0 = Original Record_x000D_
+    <t>0 = Original Record
 1 = Alias Record</t>
   </si>
   <si>
@@ -308,8 +308,8 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>M = Male_x000D_
-F = Female_x000D_
+    <t>M = Male
+F = Female
 U = Unknown</t>
   </si>
   <si>
@@ -325,7 +325,7 @@
     <t>SEX_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
+    <t>0 = Edit Passed
 1 = Edit Failed, Data Queried, and Verified</t>
   </si>
   <si>
@@ -347,11 +347,11 @@
     <t>AGETYPE</t>
   </si>
   <si>
-    <t>1 = Years_x000D_
-2 = Months_x000D_
-4 = Days_x000D_
-5 = Hours_x000D_
-6 = Minutes_x000D_
+    <t>1 = Years
+2 = Months
+4 = Days
+5 = Hours
+6 = Minutes
 9 = Unknown (not classifiable)</t>
   </si>
   <si>
@@ -370,12 +370,12 @@
     <t xml:space="preserve">AGE </t>
   </si>
   <si>
-    <t>001 - 135, 999_x000D_
-Codes: If AGETYPE = 1 then 001-135, 999_x000D_
-                                        2 then 001-011, 999_x000D_
-                                        4 then 001-027, 999_x000D_
-                                        5 then 001-023, 999_x000D_
-                                        6 then 001-059, 999_x000D_
+    <t>001 - 135, 999
+Codes: If AGETYPE = 1 then 001-135, 999
+                                        2 then 001-011, 999
+                                        4 then 001-027, 999
+                                        5 then 001-023, 999
+                                        6 then 001-059, 999
                                         9 then 999</t>
   </si>
   <si>
@@ -451,28 +451,28 @@
     <t>BPLACE_ST</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
-For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR_x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
+For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -515,28 +515,28 @@
     <t>STATEC</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
-For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
+For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -576,11 +576,11 @@
     <t>MARITAL</t>
   </si>
   <si>
-    <t>M = Married_x000D_
-A = Married but Separated_x000D_
-W = Widowed_x000D_
-D = Divorced_x000D_
-S = Never Married_x000D_
+    <t>M = Married
+A = Married but Separated
+W = Widowed
+D = Divorced
+S = Never Married
 U = Not Classifiable</t>
   </si>
   <si>
@@ -596,9 +596,9 @@
     <t>MARITAL_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
-1 = Edit Failed, Data Queried, and Verified_x000D_
-2 = Edit Failed, Data Queried, but not Verified_x000D_
+    <t>0 = Edit Passed
+1 = Edit Failed, Data Queried, and Verified
+2 = Edit Failed, Data Queried, but not Verified
 4 = Edit Failed, Query Needed</t>
   </si>
   <si>
@@ -614,13 +614,13 @@
     <t>DPLACE</t>
   </si>
   <si>
-    <t>1 = Inpatient_x000D_
-2 = Emergency Room/Outpatient_x000D_
-3 = Dead on Arrival_x000D_
-4 = Decedent's Home_x000D_
-5 = Hospice Facility_x000D_
-6 = Nursing Home/Long Term Care Facility_x000D_
-7 = Other_x000D_
+    <t>1 = Inpatient
+2 = Emergency Room/Outpatient
+3 = Dead on Arrival
+4 = Decedent's Home
+5 = Hospice Facility
+6 = Nursing Home/Long Term Care Facility
+7 = Other
 9 = Unknown</t>
   </si>
   <si>
@@ -636,7 +636,7 @@
     <t>COD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
+    <t>NCHS Instruction Manual: Part 8
 Variable description ("Contents") edited; same as NCHS "Facility Name--County"</t>
   </si>
   <si>
@@ -646,12 +646,12 @@
     <t>DISP</t>
   </si>
   <si>
-    <t>B = Burial_x000D_
-C = Cremation_x000D_
-D = Donation_x000D_
-E = Entombment_x000D_
-R = Removal from state_x000D_
-O = Other_x000D_
+    <t>B = Burial
+C = Cremation
+D = Donation
+E = Entombment
+R = Removal from state
+O = Other
 U = Unknown</t>
   </si>
   <si>
@@ -688,14 +688,14 @@
     <t>DEDUC</t>
   </si>
   <si>
-    <t>1 = 8th grade or less_x000D_
-2 = 9th through 12th grade; no diploma_x000D_
-3 = High School Graduate or GED Completed_x000D_
-4 = Some college credit, but no degree_x000D_
-5 = Associate Degree_x000D_
-6 = Bachelor's Degree_x000D_
-7 = Master's Degree_x000D_
-8 = Doctorate Degree or Professional Degree_x000D_
+    <t>1 = 8th grade or less
+2 = 9th through 12th grade; no diploma
+3 = High School Graduate or GED Completed
+4 = Some college credit, but no degree
+5 = Associate Degree
+6 = Bachelor's Degree
+7 = Master's Degree
+8 = Doctorate Degree or Professional Degree
 9 = Unknown</t>
   </si>
   <si>
@@ -711,10 +711,10 @@
     <t>DEDUC_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
-1 = Edit Failed, Data Queried, and Verified_x000D_
-2 = Edit Failed, Data Queried, but not Verified_x000D_
-3 = Edit Failed, Review Needed_x000D_
+    <t>0 = Edit Passed
+1 = Edit Failed, Data Queried, and Verified
+2 = Edit Failed, Data Queried, but not Verified
+3 = Edit Failed, Review Needed
 4 = Edit Failed, Query Needed</t>
   </si>
   <si>
@@ -730,8 +730,8 @@
     <t>DETHNIC1</t>
   </si>
   <si>
-    <t>N = No, Not Mexican_x000D_
-H = Yes, Mexican_x000D_
+    <t>N = No, Not Mexican
+H = Yes, Mexican
 U = Unknown</t>
   </si>
   <si>
@@ -750,8 +750,8 @@
     <t>DETHNIC2</t>
   </si>
   <si>
-    <t>N = No, Not Puerto Rican_x000D_
-H = Yes, Puerto Rican_x000D_
+    <t>N = No, Not Puerto Rican
+H = Yes, Puerto Rican
 U = Unknown</t>
   </si>
   <si>
@@ -764,8 +764,8 @@
     <t>DETHNIC3</t>
   </si>
   <si>
-    <t>N = No, Not Cuban_x000D_
-H = Yes, Cuban_x000D_
+    <t>N = No, Not Cuban
+H = Yes, Cuban
 U = Unknown</t>
   </si>
   <si>
@@ -778,8 +778,8 @@
     <t>DETHNIC4</t>
   </si>
   <si>
-    <t>N = No, Not other Hispanic_x000D_
-H = Yes, other Hispanic_x000D_
+    <t>N = No, Not other Hispanic
+H = Yes, other Hispanic
 U = Unknown</t>
   </si>
   <si>
@@ -804,7 +804,7 @@
     <t>RACE1</t>
   </si>
   <si>
-    <t>Y = Yes, box for race checked_x000D_
+    <t>Y = Yes, box for race checked
 N = No, box for race not checked</t>
   </si>
   <si>
@@ -1180,8 +1180,8 @@
     <t>RACE_MVR</t>
   </si>
   <si>
-    <t>R = Refused_x000D_
-S = Sought, but Unknown_x000D_
+    <t>R = Refused
+S = Sought, but Unknown
 C = Not Obtainable</t>
   </si>
   <si>
@@ -1248,8 +1248,8 @@
     <t>IDOB_YR</t>
   </si>
   <si>
-    <t>4 digit year = year of death or (year of death - 1)_x000D_
-9999 = unknown_x000D_
+    <t>4 digit year = year of death or (year of death - 1)
+9999 = unknown
 Blank</t>
   </si>
   <si>
@@ -1265,30 +1265,29 @@
     <t>BSTATE</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA_x000D_
-YC = NEW YORK CITY_x000D_
-_x000D_
-For US Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA
+YC = NEW YORK CITY
+For US Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -1874,7 +1873,7 @@
     <t>SPOUSELV</t>
   </si>
   <si>
-    <t>1=yes; 2=no; 8=unmarried; 9=unknown;_x000D_
+    <t>1=yes; 2=no; 8=unmarried; 9=unknown;
 blank if not reported</t>
   </si>
   <si>
@@ -2007,7 +2006,7 @@
     <t>RESSTATE</t>
   </si>
   <si>
-    <t>See codes used before new 2003 codes -_x000D_
+    <t>See codes used before new 2003 codes -
 Receiving state will recode</t>
   </si>
   <si>
@@ -2023,8 +2022,8 @@
     <t xml:space="preserve">DETHNICE </t>
   </si>
   <si>
-    <t>100 = NonHispanic_x000D_
-200-299 = Hispanic_x000D_
+    <t>100 = NonHispanic
+200-299 = Hispanic
 996-999 = Unknown</t>
   </si>
   <si>
@@ -2148,9 +2147,9 @@
     <t>TRANSPRT</t>
   </si>
   <si>
-    <t>DR=Driver/Operator_x000D_
-PA=Passenger_x000D_
-PE=Pedestrian_x000D_
+    <t>DR=Driver/Operator
+PA=Passenger
+PE=Pedestrian
 Enter full text if it does not fit above (blank for natural death)</t>
   </si>
   <si>
@@ -2178,7 +2177,7 @@
     <t>COUNTYCODE_I</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8; 999=unknown; _x000D_
+    <t>NCHS Instruction Manual: Part 8; 999=unknown; 
 Blank for natural death.</t>
   </si>
   <si>
@@ -2212,27 +2211,27 @@
     <t>STATECODE_I</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                 For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                 For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -2464,27 +2463,27 @@
     <t>DISPSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                  For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                  For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -2587,27 +2586,27 @@
     <t>FUNSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                       For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL NEWFOUNDLAND AND LABRADOR_x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                       For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL NEWFOUNDLAND AND LABRADOR
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -2740,27 +2739,27 @@
     <t>CERTSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                   For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL NEWFOUNDLAND AND LABRADOR_x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                   For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL NEWFOUNDLAND AND LABRADOR
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -2890,7 +2889,7 @@
     <t>MARITAL_DESCRIP</t>
   </si>
   <si>
-    <t>Free text for use of jurisdictions with domestic partnerships, other_x000D_
+    <t>Free text for use of jurisdictions with domestic partnerships, other
 types of relationships.</t>
   </si>
   <si>
@@ -3140,27 +3139,27 @@
     <t>BundleDocumentCodedCauseOfFetalDeath</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                        For US Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                        For US Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -3176,26 +3175,26 @@
     <t>State, U.S. Territory or Canadian Province of Death - literal</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -3259,28 +3258,28 @@
     <t>State, U.S. Territory or Canadian Province of Decedent's Residence - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
-For US Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL NEWFOUNDLAND AND LABRADOR _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
+For US Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL NEWFOUNDLAND AND LABRADOR 
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -3527,26 +3526,26 @@
     <t>STATE_T</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-For US Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+For US Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -3559,7 +3558,7 @@
     <t>Void Flag</t>
   </si>
   <si>
-    <t>0 = default; valid record_x000D_
+    <t>0 = default; valid record
 1 = VOID record</t>
   </si>
   <si>
@@ -3617,10 +3616,10 @@
     <t>TPLACE</t>
   </si>
   <si>
-    <t>1 = Hospital_x000D_
-2 = Clinic_x000D_
-3 = Doctor's Office_x000D_
-4 = Other_x000D_
+    <t>1 = Hospital
+2 = Clinic
+3 = Doctor's Office
+4 = Other
 9 = Unknown</t>
   </si>
   <si>
@@ -3648,7 +3647,7 @@
     <t>AGE</t>
   </si>
   <si>
-    <t>10-55_x000D_
+    <t>10-55
 99 = Unknown</t>
   </si>
   <si>
@@ -3661,27 +3660,27 @@
     <t>State, U.S. Territory or Canadian Province of Residence (Patient) - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                     For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR_x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                     For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -3751,12 +3750,12 @@
     <t>Patient's Marital Status</t>
   </si>
   <si>
-    <t>1 = Never Married_x000D_
-2 = Now Married_x000D_
-3 = Widowed_x000D_
-4 = Divorced_x000D_
-5 = Separated_x000D_
-7 = Other (specify below)_x000D_
+    <t>1 = Never Married
+2 = Now Married
+3 = Widowed
+4 = Divorced
+5 = Separated
+7 = Other (specify below)
 9 = Unknown or Not Stated</t>
   </si>
   <si>
@@ -3811,13 +3810,13 @@
     <t>ETHNIC_OLD</t>
   </si>
   <si>
-    <t>from single choice versus mark all_x000D_
-0 = non-hispanic_x000D_
-1 = Mexican_x000D_
-2 = Puerto Rican_x000D_
-3 = Cuban_x000D_
-4 = Central of South American_x000D_
-5 = Other or unknown hispanic_x000D_
+    <t>from single choice versus mark all
+0 = non-hispanic
+1 = Mexican
+2 = Puerto Rican
+3 = Cuban
+4 = Central of South American
+5 = Other or unknown hispanic
 9 = Not classifiable</t>
   </si>
   <si>
@@ -3827,15 +3826,15 @@
     <t>ETHNIC_OTH</t>
   </si>
   <si>
-    <t>Comma delimit multiple entries; _x000D_
+    <t>Comma delimit multiple entries; 
 Some states keep a version of multiple Hispanic origin that is not in the new format but something in between.</t>
   </si>
   <si>
     <t>Patient's Race--White</t>
   </si>
   <si>
-    <t>Y = Yes, box for race checked_x000D_
-N = No, box for race not checked_x000D_
+    <t>Y = Yes, box for race checked
+N = No, box for race not checked
 U = Unknown race (U in all race fields)</t>
   </si>
   <si>
@@ -3914,14 +3913,14 @@
     <t>RACE_OLD</t>
   </si>
   <si>
-    <t>From single choice versus mark all_x000D_
-1 = white; 2 =  Black;_x000D_
-3 = American Indian; 4 = Chinese_x000D_
-5 = Japanese; 6 = Hawaiian;_x000D_
-7 = Filipino; 8 = Other Asian/ Pac Islander;_x000D_
-9 = not reported; A = Asian Indian; _x000D_
-B = Korean; C = Samoan;_x000D_
-D = Vietnamese; E = Guamian;_x000D_
+    <t>From single choice versus mark all
+1 = white; 2 =  Black;
+3 = American Indian; 4 = Chinese
+5 = Japanese; 6 = Hawaiian;
+7 = Filipino; 8 = Other Asian/ Pac Islander;
+9 = not reported; A = Asian Indian; 
+B = Korean; C = Samoan;
+D = Vietnamese; E = Guamian;
 F = Multi-racial</t>
   </si>
   <si>
@@ -3931,7 +3930,7 @@
     <t>RACE_OTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma delimit multiple entries;_x000D_
+    <t xml:space="preserve">Comma delimit multiple entries;
 Some states keep a version of multiple race that is not in the new format but something in between. </t>
   </si>
   <si>
@@ -3941,7 +3940,7 @@
     <t>PREV_PREG</t>
   </si>
   <si>
-    <t>00-30_x000D_
+    <t>00-30
 99 = Unknown</t>
   </si>
   <si>
@@ -3951,14 +3950,14 @@
     <t>PLBT</t>
   </si>
   <si>
-    <t>Previous live births,_x000D_
+    <t>Previous live births,
 Now living</t>
   </si>
   <si>
     <t>PLBL</t>
   </si>
   <si>
-    <t>Previous live births,_x000D_
+    <t>Previous live births,
 Now dead</t>
   </si>
   <si>
@@ -3989,7 +3988,7 @@
     <t>DLMP_MO</t>
   </si>
   <si>
-    <t>00-12_x000D_
+    <t>00-12
 99 = Unknown</t>
   </si>
   <si>
@@ -3999,7 +3998,7 @@
     <t>DLMP_DY</t>
   </si>
   <si>
-    <t>01-31 (based on month)_x000D_
+    <t>01-31 (based on month)
 99 = Unknown</t>
   </si>
   <si>
@@ -4009,7 +4008,7 @@
     <t>CWGEST</t>
   </si>
   <si>
-    <t>01-27_x000D_
+    <t>01-27
 99 = Unknown</t>
   </si>
   <si>
@@ -4079,18 +4078,18 @@
     <t>PROC_T</t>
   </si>
   <si>
-    <t>1 = Suction Curettage_x000D_
-2 = Medical (Non-surgical; medication induced -- specify medication(s) in field below)_x000D_
-3 = Dilation &amp; Evacuation (D&amp;E)_x000D_
-4 = Intra-Uterine Instillation (Saline or Prostaglandin)_x000D_
-5 = Vaginal Prostaglandin_x000D_
-6 = Sharp Curettage (D&amp;C)_x000D_
-7 = Hysterotomy/Hysterectomy_x000D_
-8 = Other_x000D_
+    <t>1 = Suction Curettage
+2 = Medical (Non-surgical; medication induced -- specify medication(s) in field below)
+3 = Dilation &amp; Evacuation (D&amp;E)
+4 = Intra-Uterine Instillation (Saline or Prostaglandin)
+5 = Vaginal Prostaglandin
+6 = Sharp Curettage (D&amp;C)
+7 = Hysterotomy/Hysterectomy
+8 = Other
 9 = Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Medical (non-surgical) procedure medication(s) literal _x000D_
+    <t xml:space="preserve">Medical (non-surgical) procedure medication(s) literal 
 </t>
   </si>
   <si>
@@ -4100,7 +4099,7 @@
     <t>Free form literal specifing medication(s) that terminated this pregnancy.</t>
   </si>
   <si>
-    <t xml:space="preserve">Termination other procedure literal _x000D_
+    <t xml:space="preserve">Termination other procedure literal 
 </t>
   </si>
   <si>
@@ -4116,15 +4115,15 @@
     <t>PROC-OTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeat up to 4 single digit codes                            _x000D_
-0 = None                                                                                                                                                                                                                           1 = Suction Curettage_x000D_
-2 = Medical (Non-surgical; medication induced)_x000D_
-3 = Dilation &amp; Evacuation (D&amp;E)_x000D_
-4 = Intra-Uterine Instillation (Saline or Prostaglandin)_x000D_
-5 = Vaginal Prostaglandin_x000D_
-6 = Sharp Curettage (D&amp;C)_x000D_
-8 = Other_x000D_
-9 = Unknown_x000D_
+    <t xml:space="preserve">Repeat up to 4 single digit codes                            
+0 = None                                                                                                                                                                                                                           1 = Suction Curettage
+2 = Medical (Non-surgical; medication induced)
+3 = Dilation &amp; Evacuation (D&amp;E)
+4 = Intra-Uterine Instillation (Saline or Prostaglandin)
+5 = Vaginal Prostaglandin
+6 = Sharp Curettage (D&amp;C)
+8 = Other
+9 = Unknown
 </t>
   </si>
   <si>
@@ -4134,7 +4133,7 @@
     <t>CALC_WGEST</t>
   </si>
   <si>
-    <t>00-95_x000D_
+    <t>00-95
 99 = Unknown</t>
   </si>
   <si>
@@ -4147,7 +4146,7 @@
     <t>Y, N, or U (if N or U, leave all other TP complications blank)</t>
   </si>
   <si>
-    <t>Hemorrhage_x000D_
+    <t>Hemorrhage
 (at time of procedure)</t>
   </si>
   <si>
@@ -4157,56 +4156,56 @@
     <t>Y, N, U (some jurisdictions may only collect hemorage data if above a certain volumn)</t>
   </si>
   <si>
-    <t>Infection_x000D_
+    <t>Infection
 (at time of procedure)</t>
   </si>
   <si>
     <t>INFECT_TP</t>
   </si>
   <si>
-    <t>Uterine perforation_x000D_
+    <t>Uterine perforation
 (at time of procedure)</t>
   </si>
   <si>
     <t>PERF_TP</t>
   </si>
   <si>
-    <t>Cervical laceration_x000D_
+    <t>Cervical laceration
 (at time of procedure)</t>
   </si>
   <si>
     <t>LACER_TP</t>
   </si>
   <si>
-    <t>Retained products_x000D_
+    <t>Retained products
 (at time of procedure)</t>
   </si>
   <si>
     <t>RETAN_TP</t>
   </si>
   <si>
-    <t>Death _x000D_
+    <t>Death 
 (at time of procedure)</t>
   </si>
   <si>
     <t>DEATH_TP</t>
   </si>
   <si>
-    <t>Failure of first method _x000D_
+    <t>Failure of first method 
 (at time of procedure)</t>
   </si>
   <si>
     <t>FAIL_TP</t>
   </si>
   <si>
-    <t>Other complications _x000D_
+    <t>Other complications 
 (at time of procedure)</t>
   </si>
   <si>
     <t>OTHER_TP</t>
   </si>
   <si>
-    <t>Other complications literal _x000D_
+    <t>Other complications literal 
 (at time of procedure)</t>
   </si>
   <si>
@@ -4225,49 +4224,49 @@
     <t>Y, N, or U (if N or U, leave all other F1 complications blank)</t>
   </si>
   <si>
-    <t>Complications at followup_x000D_
+    <t>Complications at followup
 at same facility</t>
   </si>
   <si>
     <t>COMP_F1</t>
   </si>
   <si>
-    <t>Hemorrhage_x000D_
+    <t>Hemorrhage
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>HEMOR_F1</t>
   </si>
   <si>
-    <t>Infection _x000D_
+    <t>Infection 
 (at time of  follow up at this facility)</t>
   </si>
   <si>
     <t>INFECT_F1</t>
   </si>
   <si>
-    <t>Uterine perforation _x000D_
+    <t>Uterine perforation 
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>PERF_F1</t>
   </si>
   <si>
-    <t>Cervical laceration _x000D_
+    <t>Cervical laceration 
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>LACER_F1</t>
   </si>
   <si>
-    <t>Retained products _x000D_
+    <t>Retained products 
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>RETAN_F1</t>
   </si>
   <si>
-    <t>Death _x000D_
+    <t>Death 
 (at time of followup at this facility)</t>
   </si>
   <si>
@@ -4286,7 +4285,7 @@
     <t>OTHER_F1</t>
   </si>
   <si>
-    <t>Other complications literal _x000D_
+    <t>Other complications literal 
 (at time of followup at this facility)</t>
   </si>
   <si>
@@ -4305,70 +4304,70 @@
     <t>Y, N, or U (if N or U, leave all other F2 complications blank)</t>
   </si>
   <si>
-    <t>Complications _x000D_
+    <t>Complications 
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>COMP_F2</t>
   </si>
   <si>
-    <t>Hemorrhage_x000D_
+    <t>Hemorrhage
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>HEMOR_F2</t>
   </si>
   <si>
-    <t>Infection _x000D_
+    <t>Infection 
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>INFECT_F2</t>
   </si>
   <si>
-    <t>Uterine perforation  _x000D_
+    <t>Uterine perforation  
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>PERF_F2</t>
   </si>
   <si>
-    <t>Cervical laceration  _x000D_
+    <t>Cervical laceration  
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>LACER_F2</t>
   </si>
   <si>
-    <t>Retained products _x000D_
+    <t>Retained products 
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>RETAN_F2</t>
   </si>
   <si>
-    <t>Death _x000D_
+    <t>Death 
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>DEATH_F2</t>
   </si>
   <si>
-    <t>Failure of first method _x000D_
+    <t>Failure of first method 
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>FAIL_F2</t>
   </si>
   <si>
-    <t xml:space="preserve">Other complications _x000D_
+    <t xml:space="preserve">Other complications 
 (at time of followup at other facility) </t>
   </si>
   <si>
     <t>OTHER_F2</t>
   </si>
   <si>
-    <t>Other complications literal _x000D_
+    <t>Other complications literal 
 (at time of followup at other facility)</t>
   </si>
   <si>
@@ -4378,17 +4377,17 @@
     <t>Free form literal of specified other complication at time of followup at other facility.</t>
   </si>
   <si>
-    <t>Site of follow-up visit _x000D_
+    <t>Site of follow-up visit 
 (at other facility)</t>
   </si>
   <si>
     <t>SITE_F2</t>
   </si>
   <si>
-    <t>1 = physician's office_x000D_
-2 = clinic_x000D_
-3 = hospital_x000D_
-4 = other, specify_x000D_
+    <t>1 = physician's office
+2 = clinic
+3 = hospital
+4 = other, specify
 9 = unknown</t>
   </si>
   <si>
@@ -4698,13 +4697,13 @@
     <t>Place Where Delivery Occurred</t>
   </si>
   <si>
-    <t>1 = Hospital_x000D_
-2 = Freestanding Birth Center_x000D_
-3 = Home (Intended)_x000D_
-4 = Home (Not Intended)_x000D_
-5 = Home (Unknown if Intended)_x000D_
-6 = Clinic/Doctor's Office_x000D_
-7 = Other_x000D_
+    <t>1 = Hospital
+2 = Freestanding Birth Center
+3 = Home (Intended)
+4 = Home (Not Intended)
+5 = Home (Unknown if Intended)
+6 = Clinic/Doctor's Office
+7 = Other
 9 = Unknown</t>
   </si>
   <si>
@@ -4762,7 +4761,7 @@
     <t>MAGE_BYPASS</t>
   </si>
   <si>
-    <t xml:space="preserve">0 = Edit Passed_x000D_
+    <t xml:space="preserve">0 = Edit Passed
 1 = Data Queried </t>
   </si>
   <si>
@@ -4781,27 +4780,27 @@
     <t>BPLACEC_ST_TER</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -4826,27 +4825,27 @@
     <t>State, U.S. Territory or Canadian Province of Residence (Mother) - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR_x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -4856,8 +4855,8 @@
     <t>Residence of Mother--Inside City/Town Limits</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
+    <t>Y = Yes
+N = No
 U = Unknown</t>
   </si>
   <si>
@@ -4927,8 +4926,8 @@
     <t>MEDUC_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
-1 = Edit Failed, Data Queried and Verified_x000D_
+    <t>0 = Edit Passed
+1 = Edit Failed, Data Queried and Verified
 2 = Edit Failed, Data Queried, but not Verified</t>
   </si>
   <si>
@@ -5349,11 +5348,11 @@
     <t>ATTEND</t>
   </si>
   <si>
-    <t>1 = MD_x000D_
-2 = DO_x000D_
-3 = CNM/CM_x000D_
-4 = Other midwife_x000D_
-5 = Other (specify)_x000D_
+    <t>1 = MD
+2 = DO
+3 = CNM/CM
+4 = Other midwife
+5 = Other (specify)
 9 = Unknown</t>
   </si>
   <si>
@@ -5402,7 +5401,7 @@
     <t>DOFP_YR</t>
   </si>
   <si>
-    <t>4 digit year; year of delivery or_x000D_
+    <t>4 digit year; year of delivery or
 (year of delivery - 1), 8888, 9999</t>
   </si>
   <si>
@@ -5439,8 +5438,8 @@
     <t>NPREV_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
-1 = Edit Failed, Number Verified_x000D_
+    <t>0 = Edit Passed
+1 = Edit Failed, Number Verified
 2 = Edit Failed, Number not Verified</t>
   </si>
   <si>
@@ -5474,8 +5473,8 @@
     <t>HGT_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
-1 = Edit Failed, Number Verified_x000D_
+    <t>0 = Edit Passed
+1 = Edit Failed, Number Verified
 2 = Edit Failed, Number not  Verified</t>
   </si>
   <si>
@@ -5503,8 +5502,8 @@
     <t>PWGT_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
-1 = Edit Failed, Verified_x000D_
+    <t>0 = Edit Passed
+1 = Edit Failed, Verified
 2 = Edit Failed, not Verified</t>
   </si>
   <si>
@@ -5571,8 +5570,8 @@
     <t>YLLB</t>
   </si>
   <si>
-    <t>4 digit year;_x000D_
-(year of mother's birth + 10) through_x000D_
+    <t>4 digit year;
+(year of mother's birth + 10) through
 year of delivery, 8888, 9999</t>
   </si>
   <si>
@@ -5630,8 +5629,8 @@
     <t>Date Last Normal Menses Began--Year</t>
   </si>
   <si>
-    <t>4 digit year; year of delivery or_x000D_
-(year of delivery - 1) or_x000D_
+    <t>4 digit year; year of delivery or
+(year of delivery - 1) or
 (year of delivery - 2), 9999</t>
   </si>
   <si>
@@ -5656,9 +5655,9 @@
     <t>See [note on missing pregnancy risk factors data]</t>
   </si>
   <si>
-    <t>Update risk factors (old Observation-pregnancy-risk-factor)_x000D_
-STU 1 listed:_x000D_
-IJE Natality Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART_x000D_
+    <t>Update risk factors (old Observation-pregnancy-risk-factor)
+STU 1 listed:
+IJE Natality Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART
 IJE Fetal Death Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART</t>
   </si>
   <si>
@@ -5749,7 +5748,7 @@
     <t>NPCES_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
+    <t>0 = Edit Passed
 1 = Edit Failed, Verified</t>
   </si>
   <si>
@@ -5837,9 +5836,9 @@
     <t>PRES</t>
   </si>
   <si>
-    <t>1 = Cephalic_x000D_
-2 = Breech_x000D_
-3 = Other_x000D_
+    <t>1 = Cephalic
+2 = Breech
+3 = Other
 9 = Unknown</t>
   </si>
   <si>
@@ -5855,10 +5854,10 @@
     <t>ROUT</t>
   </si>
   <si>
-    <t>1 = Spontaneous_x000D_
-2 = Forceps_x000D_
-3 = Vacuum_x000D_
-4 = Cesarean_x000D_
+    <t>1 = Spontaneous
+2 = Forceps
+3 = Vacuum
+4 = Cesarean
 9 = Unknown</t>
   </si>
   <si>
@@ -5877,9 +5876,9 @@
     <t>TLAB</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
-U = Unknown_x000D_
+    <t>Y = Yes
+N = No
+U = Unknown
 X = Not Applicable</t>
   </si>
   <si>
@@ -5898,9 +5897,9 @@
     <t>MTR</t>
   </si>
   <si>
-    <t>Update maternal morbidity (old Condition-maternal-morbidity)_x000D_
-STU 1 listed:_x000D_
-IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT_x000D_
+    <t>Update maternal morbidity (old Condition-maternal-morbidity)
+STU 1 listed:
+IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT
 IJE Fetal Death Data Elements: RUT, AINT</t>
   </si>
   <si>
@@ -5949,10 +5948,10 @@
     <t>UOPR</t>
   </si>
   <si>
-    <t>Update maternal morbidity (old Condition-maternal-morbidity)_x000D_
-STU 1 listed:_x000D_
-IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT_x000D_
-IJE Fetal Death Data Elements: RUT, AINT_x000D_
+    <t>Update maternal morbidity (old Condition-maternal-morbidity)
+STU 1 listed:
+IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT
+IJE Fetal Death Data Elements: RUT, AINT
 (new) UOPR</t>
   </si>
   <si>
@@ -5971,8 +5970,8 @@
     <t>FW_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off_x000D_
-1 = Queried data correct, out of range_x000D_
+    <t>0 = Off
+1 = Queried data correct, out of range
 2 = Queried, failed  delivery weight/gestation edit</t>
   </si>
   <si>
@@ -5994,7 +5993,7 @@
     <t>OWGEST_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off_x000D_
+    <t>0 = Off
 1 = Queried data correct, out of range</t>
   </si>
   <si>
@@ -6007,9 +6006,9 @@
     <t>ETIME</t>
   </si>
   <si>
-    <t>N = At assessment, no labor_x000D_
-L = At assessment, labor_x000D_
-A = Labor, no assessment_x000D_
+    <t>N = At assessment, no labor
+L = At assessment, labor
+A = Labor, no assessment
 U = Unknown</t>
   </si>
   <si>
@@ -6022,8 +6021,8 @@
     <t>Was an Autopsy Performed?</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
+    <t>Y = Yes
+N = No
 P = Planned</t>
   </si>
   <si>
@@ -6045,8 +6044,8 @@
     <t>Were Autopsy or Histological Placental Examination Results Used in Determining the Cause of Fetal Death?</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
+    <t>Y = Yes
+N = No
 X = Not Applicable</t>
   </si>
   <si>
@@ -6095,8 +6094,8 @@
     <t>PLUR_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off_x000D_
-1 = Queried, and Correct_x000D_
+    <t>0 = Off
+1 = Queried, and Correct
 2 = Plurality/Set Order Queried, Inconsistent</t>
   </si>
   <si>
@@ -6166,9 +6165,9 @@
     <t>DOWT</t>
   </si>
   <si>
-    <t>C = Confirmed_x000D_
-P = Pending_x000D_
-N = No_x000D_
+    <t>C = Confirmed
+P = Pending
+N = No
 U = Unknown</t>
   </si>
   <si>
@@ -6190,10 +6189,10 @@
     <t>&gt;=year of delivery</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
-Code structure description differs here_x000D_
-Code sent back to state VRO_x000D_
-For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
+    <t>Code used on 3 tabs: N, FD, &amp; BID
+Code structure description differs here
+Code sent back to state VRO
+For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -6209,10 +6208,10 @@
     <t>NCHS USE ONLY: Receipt date -- Day</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
-Code structure description differs here_x000D_
-Code sent back to state VRO_x000D_
-Note: Marked as NCHS USE ONLY, but VRDR does address this. For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
+    <t>Code used on 3 tabs: N, FD, &amp; BID
+Code structure description differs here
+Code sent back to state VRO
+Note: Marked as NCHS USE ONLY, but VRDR does address this. For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -6255,9 +6254,9 @@
     <t>INFT_DRG</t>
   </si>
   <si>
-    <t>Y = Yes (BLANK IF NOT ADDED)_x000D_
-N = No_x000D_
-X = Not Applicable_x000D_
+    <t>Y = Yes (BLANK IF NOT ADDED)
+N = No
+X = Not Applicable
 U = Unknown</t>
   </si>
   <si>
@@ -6294,7 +6293,7 @@
     <t>COD18a1</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
+    <t>Y = Yes
 N = No</t>
   </si>
   <si>
@@ -6979,9 +6978,9 @@
     <t>string(25)</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
-NCHS does not use_x000D_
-VRCL defines "ObservationUsualWorkVitalRecords" profile. _x000D_
+    <t>Code used on 3 tabs: N, FD, &amp; BID
+NCHS does not use
+VRCL defines "ObservationUsualWorkVitalRecords" profile. 
 Decision: BFDR should mimic VRDR</t>
   </si>
   <si>
@@ -7543,24 +7542,24 @@
     <t>MRACEBG_C</t>
   </si>
   <si>
-    <t>01 = White_x000D_
-02 = Black_x000D_
-03 = American Indian/Alaskan Native_x000D_
-04 = Asian Indian_x000D_
-05 = Chinese_x000D_
-06 = Filipino_x000D_
-07 = Japanese_x000D_
-08 = Korean_x000D_
-09 = Vietnamese_x000D_
-10 = Other Asian_x000D_
-11 = Native Hawaiian_x000D_
-12 = Guamanian_x000D_
-13 = Samoan_x000D_
-14 = Other Pacific Islander_x000D_
-15 = Other_x000D_
-21 = Bridged White_x000D_
-22 = Bridged Black_x000D_
-23 = Bridged American Indian/Alaskan Native_x000D_
+    <t>01 = White
+02 = Black
+03 = American Indian/Alaskan Native
+04 = Asian Indian
+05 = Chinese
+06 = Filipino
+07 = Japanese
+08 = Korean
+09 = Vietnamese
+10 = Other Asian
+11 = Native Hawaiian
+12 = Guamanian
+13 = Samoan
+14 = Other Pacific Islander
+15 = Other
+21 = Bridged White
+22 = Bridged Black
+23 = Bridged American Indian/Alaskan Native
 24 = Bridged Asian &amp; Pacific Islander</t>
   </si>
   <si>
@@ -7681,24 +7680,24 @@
     <t>Informant's Relationship to Fetus</t>
   </si>
   <si>
-    <t>1 = Mother_x000D_
-2 = Father_x000D_
-3 = Sibling_x000D_
-4 = Other relative_x000D_
-5 = Other_x000D_
+    <t>1 = Mother
+2 = Father
+3 = Sibling
+4 = Other relative
+5 = Other
 9 = Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Only similar item is Mortality: "Informant's Relationship (INFORMRELATE), which uses VRDR Decedent  contact.type.text   string (30 characters)_x000D_
-VRCPL has:_x000D_
-  - Patient-decedent-fetus, _x000D_
-  - Related Person - Parent Vital Records   _x000D_
-  - RelatedPerson - Father Natural Vital Records         _x000D_
-  - RelatedPerson - Father Vital Records         _x000D_
-  - RelatedPerson - Mother Gestational Vital Records         _x000D_
-  - RelatedPerson - Mother Vital Records_x000D_
-NOTE that the IJE Code Structure Description here includes Sibling and others_x000D_
-Saul notes: VRDR uses fields that can be from a controlled vocabulary or any arbitrary string (e.g., CERTL in  http://build.fhir.org/ig/HL7/vrdr/branches/master/StructureDefinition-vrdr-death-certification.html) with a consistent pattern (I think_x000D_
+    <t xml:space="preserve">Only similar item is Mortality: "Informant's Relationship (INFORMRELATE), which uses VRDR Decedent  contact.type.text   string (30 characters)
+VRCPL has:
+  - Patient-decedent-fetus, 
+  - Related Person - Parent Vital Records   
+  - RelatedPerson - Father Natural Vital Records         
+  - RelatedPerson - Father Vital Records         
+  - RelatedPerson - Mother Gestational Vital Records         
+  - RelatedPerson - Mother Vital Records
+NOTE that the IJE Code Structure Description here includes Sibling and others
+Saul notes: VRDR uses fields that can be from a controlled vocabulary or any arbitrary string (e.g., CERTL in  http://build.fhir.org/ig/HL7/vrdr/branches/master/StructureDefinition-vrdr-death-certification.html) with a consistent pattern (I think
 there are two such fields). </t>
   </si>
   <si>
@@ -7753,9 +7752,9 @@
     <t>Deprecated, see [VRFM]</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
-Mortality (VRDR) uses   DeathCertificate  extension[replaceStatus].valuecodeable   [ReplaceStatusVS]_x000D_
-VRDR addresses in the VRDR Messaging IG. _x000D_
+    <t>Code used on 3 tabs: N, FD, &amp; BID
+Mortality (VRDR) uses   DeathCertificate  extension[replaceStatus].valuecodeable   [ReplaceStatusVS]
+VRDR addresses in the VRDR Messaging IG. 
 Decision: Births should behave the same as deaths.</t>
   </si>
   <si>
@@ -7771,31 +7770,30 @@
     <t>State, U.S. Territory or Canadian Province of Birth (Infant) - code</t>
   </si>
   <si>
-    <t>_x000D_
-NCHS Instruction Manual: Part 8_x000D_
-ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA_x000D_
-YC = NEW YORK CITY_x000D_
-_x000D_
-For US Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t xml:space="preserve">
+NCHS Instruction Manual: Part 8
+ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA
+YC = NEW YORK CITY
+For US Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -7817,8 +7815,8 @@
     <t>ISEX</t>
   </si>
   <si>
-    <t>M = Male_x000D_
-F = Female_x000D_
+    <t>M = Male
+F = Female
 N = Not Yet Determined</t>
   </si>
   <si>
@@ -7852,31 +7850,31 @@
     <t>4 digit year (&lt; year of birth of child);  9999 = unknown</t>
   </si>
   <si>
-    <t>0 = Edit Passed_x000D_
+    <t>0 = Edit Passed
 1 = Data Queried</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR 
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -7886,27 +7884,27 @@
     <t>Residence of Mother--City</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA        For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA        For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR 
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -7946,15 +7944,15 @@
     <t>Literal; blank</t>
   </si>
   <si>
-    <t xml:space="preserve">NCHS Appendix E_x000D_
-(values for fields 62 - 77 returned from NCHS)_x000D_
+    <t xml:space="preserve">NCHS Appendix E
+(values for fields 62 - 77 returned from NCHS)
 </t>
   </si>
   <si>
     <t>NCHS Appendix E</t>
   </si>
   <si>
-    <t>NCHS Appendix E_x000D_
+    <t>NCHS Appendix E
 (values for fields 108 - 123 returned from NCHS)</t>
   </si>
   <si>
@@ -7976,11 +7974,11 @@
     <t>01-31 (based on month), 88=no care, 99=unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">4 digit year; year of child's birth or_x000D_
+    <t xml:space="preserve">4 digit year; year of child's birth or
 (year of child's birth - 1), 8888=no care, 9999=unknown </t>
   </si>
   <si>
-    <t>4 digit year; year of child's birth or _x000D_
+    <t>4 digit year; year of child's birth or 
 (year of child's birth - 1), 8888=no care, 9999=unknown</t>
   </si>
   <si>
@@ -8011,7 +8009,7 @@
     <t>ObservationNumberOtherPregnancyOutcomes</t>
   </si>
   <si>
-    <t>4 digit year;(year of mother's birth + 10) through_x000D_
+    <t>4 digit year;(year of mother's birth + 10) through
 year of child's birth, 8888, 9999</t>
   </si>
   <si>
@@ -8033,13 +8031,13 @@
     <t>PAY</t>
   </si>
   <si>
-    <t>1 = Medicaid_x000D_
-2 = Private Insurance_x000D_
-3 = Self-pay_x000D_
-4 = Indian Health Service_x000D_
-5 = CHAMPUS/TRICARE_x000D_
-6 = Other Government (Fed, State, Local) _x000D_
-8 = Other_x000D_
+    <t>1 = Medicaid
+2 = Private Insurance
+3 = Self-pay
+4 = Indian Health Service
+5 = CHAMPUS/TRICARE
+6 = Other Government (Fed, State, Local) 
+8 = Other
 9 = Unknown</t>
   </si>
   <si>
@@ -8052,8 +8050,8 @@
     <t>[BirthAndFetalDeathFinancialClassVS] </t>
   </si>
   <si>
-    <t>4 digit year; year of child's birth _x000D_
-or (year of child's birth - 1)_x000D_
+    <t>4 digit year; year of child's birth 
+or (year of child's birth - 1)
 or (year of child's birth - 2), 9999</t>
   </si>
   <si>
@@ -8186,8 +8184,8 @@
     <t>See [note on missing characteristics of labor and delivery data]</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
-STU 1 listed:_x000D_
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
+STU 1 listed:
 IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN</t>
   </si>
   <si>
@@ -8242,9 +8240,9 @@
     <t>MECS</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
-STU 1 listed:_x000D_
-IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN_x000D_
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
+STU 1 listed:
+IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN
 (new) MECS</t>
   </si>
   <si>
@@ -8254,9 +8252,9 @@
     <t>FINT</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
-STU 1 listed:_x000D_
-IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN_x000D_
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
+STU 1 listed:
+IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN
 (new) FINT</t>
   </si>
   <si>
@@ -8302,8 +8300,8 @@
     <t>BW_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off_x000D_
-1 = Queried data correct, out of range_x000D_
+    <t>0 = Off
+1 = Queried data correct, out of range
 2 = Queried, failed birthweight/gestation edit</t>
   </si>
   <si>
@@ -8343,8 +8341,8 @@
     <t>ObservationNumberLiveBirthsThisDelivery</t>
   </si>
   <si>
-    <t>0 = OFF_x000D_
-1 = Queried, and Correct_x000D_
+    <t>0 = OFF
+1 = Queried, and Correct
 2 = Plurality/Set Order Queried, Inconsistent</t>
   </si>
   <si>
@@ -8360,8 +8358,8 @@
     <t>See [note on missing abnormal conditions of newborn data]</t>
   </si>
   <si>
-    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)_x000D_
-STU 1 listed:_x000D_
+    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)
+STU 1 listed:
 IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH</t>
   </si>
   <si>
@@ -8419,9 +8417,9 @@
     <t>BINJ</t>
   </si>
   <si>
-    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)_x000D_
-STU 1 listed:_x000D_
-IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH_x000D_
+    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)
+STU 1 listed:
+IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH
 (new) BINJ</t>
   </si>
   <si>
@@ -8521,8 +8519,8 @@
     <t>ILIV</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
+    <t>Y = Yes
+N = No
 U = Infant transferred, Status Unknown</t>
   </si>
   <si>
@@ -8541,9 +8539,9 @@
     <t>leave blank</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
-Code sent back to state VRO_x000D_
-For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
+    <t>Code used on 3 tabs: N, FD, &amp; BID
+Code sent back to state VRO
+For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -8553,10 +8551,10 @@
     <t>Risk Factors--Infertility: Fertility Enhancing Drugs  (RECOMMENDED ADDITION EFFECTIVE 2004)</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
-X = Not Applicable_x000D_
-U = Unknown_x000D_
+    <t>Y = Yes
+N = No
+X = Not Applicable
+U = Unknown
 (BLANK IF NOT ADDED)</t>
   </si>
   <si>
@@ -8713,27 +8711,27 @@
     <t>Refer to NCHS Instruction Manual Part 19, Industry and Occupation Coding for Death Certificates, 2003. Leave blank if using a coding system other than this</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -8857,8 +8855,8 @@
     <t>SSN_MULT_BTH_CD</t>
   </si>
   <si>
-    <t>Y = Yes_x000D_
-N = No_x000D_
+    <t>Y = Yes
+N = No
 or blank</t>
   </si>
   <si>
@@ -8907,12 +8905,12 @@
     <t>CERTIF</t>
   </si>
   <si>
-    <t>1 = MD_x000D_
-2 = DO_x000D_
-3 = CNM/CM_x000D_
-4 = Other midwife_x000D_
-5 = Other (specify) _x000D_
-6 = Hospital Admin_x000D_
+    <t>1 = MD
+2 = DO
+3 = CNM/CM
+4 = Other midwife
+5 = Other (specify) 
+6 = Hospital Admin
 9 = Unknown</t>
   </si>
   <si>
@@ -8961,51 +8959,51 @@
     <t>Deprecated,  see [VRFM]</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA              For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA              For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR 
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8_x000D_
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA            For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
-For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual: Part 8
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA            For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR 
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>
@@ -9081,7 +9079,7 @@
     <t>Residence Street number</t>
   </si>
   <si>
-    <t>For use of jurisdictions with domestic partnerships, other_x000D_
+    <t>For use of jurisdictions with domestic partnerships, other
 types of relationships.</t>
   </si>
   <si>
@@ -9106,26 +9104,26 @@
     <t>Death Jurisdiction - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual Part 8A_x000D_
- For U.S. Territories:_x000D_
-   MP  NORTHERN MARIANAS_x000D_
-   AS  AMERICAN SAMOA_x000D_
-   GU  GUAM_x000D_
-   VI   VIRGIN ISLANDS_x000D_
-   PR  PUERTO RICO_x000D_
- For Canadian Provinces:_x000D_
-   AB  ALBERTA  _x000D_
-   BC  BRITISH COLUMBIA _x000D_
-   MB  MANITOBA _x000D_
-   NB  NEW BRUNSWICK  _x000D_
-   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
-   NS  NOVA SCOTIA _x000D_
-   NT  NORTHWEST TERRITORIES_x000D_
-   NU  NUNAVUT_x000D_
-   ON  ONTARIO_x000D_
-   PE  PRINCE EDWARD ISLAND _x000D_
-   QC  QUEBEC  _x000D_
-   SK  SASKATCHEWAN_x000D_
+    <t>NCHS Instruction Manual Part 8A
+ For U.S. Territories:
+   MP  NORTHERN MARIANAS
+   AS  AMERICAN SAMOA
+   GU  GUAM
+   VI   VIRGIN ISLANDS
+   PR  PUERTO RICO
+ For Canadian Provinces:
+   AB  ALBERTA  
+   BC  BRITISH COLUMBIA 
+   MB  MANITOBA 
+   NB  NEW BRUNSWICK  
+   NL  NEWFOUNDLAND AND LABRADOR  
+   NS  NOVA SCOTIA 
+   NT  NORTHWEST TERRITORIES
+   NU  NUNAVUT
+   ON  ONTARIO
+   PE  PRINCE EDWARD ISLAND 
+   QC  QUEBEC  
+   SK  SASKATCHEWAN
    YT  YUKON</t>
   </si>
   <si>

</xml_diff>

<commit_message>
adding gender note link
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -125,26 +125,26 @@
     <t>DSTATE</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -214,7 +214,7 @@
     <t>VOID</t>
   </si>
   <si>
-    <t>0 =Default; Valid Record
+    <t>0 =Default; Valid Record_x000D_
 1 = VOID record</t>
   </si>
   <si>
@@ -251,8 +251,8 @@
     <t>MFILED</t>
   </si>
   <si>
-    <t>0 = Electronic Mode
-1 = Paper Mode
+    <t>0 = Electronic Mode_x000D_
+1 = Paper Mode_x000D_
 2 = Mixed Mode</t>
   </si>
   <si>
@@ -316,7 +316,7 @@
     <t>ALIAS</t>
   </si>
   <si>
-    <t>0 = Original Record
+    <t>0 = Original Record_x000D_
 1 = Alias Record</t>
   </si>
   <si>
@@ -341,8 +341,8 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>M = Male
-F = Female
+    <t>M = Male_x000D_
+F = Female_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -358,7 +358,7 @@
     <t>SEX_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
+    <t>0 = Edit Passed_x000D_
 1 = Edit Failed, Data Queried, and Verified</t>
   </si>
   <si>
@@ -380,11 +380,11 @@
     <t>AGETYPE</t>
   </si>
   <si>
-    <t>1 = Years
-2 = Months
-4 = Days
-5 = Hours
-6 = Minutes
+    <t>1 = Years_x000D_
+2 = Months_x000D_
+4 = Days_x000D_
+5 = Hours_x000D_
+6 = Minutes_x000D_
 9 = Unknown (not classifiable)</t>
   </si>
   <si>
@@ -403,12 +403,12 @@
     <t xml:space="preserve">AGE </t>
   </si>
   <si>
-    <t>001 - 135, 999
-Codes: If AGETYPE = 1 then 001-135, 999
-                                        2 then 001-011, 999
-                                        4 then 001-027, 999
-                                        5 then 001-023, 999
-                                        6 then 001-059, 999
+    <t>001 - 135, 999_x000D_
+Codes: If AGETYPE = 1 then 001-135, 999_x000D_
+                                        2 then 001-011, 999_x000D_
+                                        4 then 001-027, 999_x000D_
+                                        5 then 001-023, 999_x000D_
+                                        6 then 001-059, 999_x000D_
                                         9 then 999</t>
   </si>
   <si>
@@ -484,28 +484,28 @@
     <t>BPLACE_ST</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -548,28 +548,28 @@
     <t>STATEC</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -609,11 +609,11 @@
     <t>MARITAL</t>
   </si>
   <si>
-    <t>M = Married
-A = Married but Separated
-W = Widowed
-D = Divorced
-S = Never Married
+    <t>M = Married_x000D_
+A = Married but Separated_x000D_
+W = Widowed_x000D_
+D = Divorced_x000D_
+S = Never Married_x000D_
 U = Not Classifiable</t>
   </si>
   <si>
@@ -629,9 +629,9 @@
     <t>MARITAL_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Data Queried, and Verified
-2 = Edit Failed, Data Queried, but not Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Data Queried, and Verified_x000D_
+2 = Edit Failed, Data Queried, but not Verified_x000D_
 4 = Edit Failed, Query Needed</t>
   </si>
   <si>
@@ -647,13 +647,13 @@
     <t>DPLACE</t>
   </si>
   <si>
-    <t>1 = Inpatient
-2 = Emergency Room/Outpatient
-3 = Dead on Arrival
-4 = Decedent's Home
-5 = Hospice Facility
-6 = Nursing Home/Long Term Care Facility
-7 = Other
+    <t>1 = Inpatient_x000D_
+2 = Emergency Room/Outpatient_x000D_
+3 = Dead on Arrival_x000D_
+4 = Decedent's Home_x000D_
+5 = Hospice Facility_x000D_
+6 = Nursing Home/Long Term Care Facility_x000D_
+7 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -669,7 +669,7 @@
     <t>COD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
+    <t>NCHS Instruction Manual: Part 8_x000D_
 Variable description ("Contents") edited; same as NCHS "Facility Name--County"</t>
   </si>
   <si>
@@ -679,12 +679,12 @@
     <t>DISP</t>
   </si>
   <si>
-    <t>B = Burial
-C = Cremation
-D = Donation
-E = Entombment
-R = Removal from state
-O = Other
+    <t>B = Burial_x000D_
+C = Cremation_x000D_
+D = Donation_x000D_
+E = Entombment_x000D_
+R = Removal from state_x000D_
+O = Other_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -721,14 +721,14 @@
     <t>DEDUC</t>
   </si>
   <si>
-    <t>1 = 8th grade or less
-2 = 9th through 12th grade; no diploma
-3 = High School Graduate or GED Completed
-4 = Some college credit, but no degree
-5 = Associate Degree
-6 = Bachelor's Degree
-7 = Master's Degree
-8 = Doctorate Degree or Professional Degree
+    <t>1 = 8th grade or less_x000D_
+2 = 9th through 12th grade; no diploma_x000D_
+3 = High School Graduate or GED Completed_x000D_
+4 = Some college credit, but no degree_x000D_
+5 = Associate Degree_x000D_
+6 = Bachelor's Degree_x000D_
+7 = Master's Degree_x000D_
+8 = Doctorate Degree or Professional Degree_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -744,10 +744,10 @@
     <t>DEDUC_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Data Queried, and Verified
-2 = Edit Failed, Data Queried, but not Verified
-3 = Edit Failed, Review Needed
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Data Queried, and Verified_x000D_
+2 = Edit Failed, Data Queried, but not Verified_x000D_
+3 = Edit Failed, Review Needed_x000D_
 4 = Edit Failed, Query Needed</t>
   </si>
   <si>
@@ -763,8 +763,8 @@
     <t>DETHNIC1</t>
   </si>
   <si>
-    <t>N = No, Not Mexican
-H = Yes, Mexican
+    <t>N = No, Not Mexican_x000D_
+H = Yes, Mexican_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -783,8 +783,8 @@
     <t>DETHNIC2</t>
   </si>
   <si>
-    <t>N = No, Not Puerto Rican
-H = Yes, Puerto Rican
+    <t>N = No, Not Puerto Rican_x000D_
+H = Yes, Puerto Rican_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -797,8 +797,8 @@
     <t>DETHNIC3</t>
   </si>
   <si>
-    <t>N = No, Not Cuban
-H = Yes, Cuban
+    <t>N = No, Not Cuban_x000D_
+H = Yes, Cuban_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -811,8 +811,8 @@
     <t>DETHNIC4</t>
   </si>
   <si>
-    <t>N = No, Not other Hispanic
-H = Yes, other Hispanic
+    <t>N = No, Not other Hispanic_x000D_
+H = Yes, other Hispanic_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -837,7 +837,7 @@
     <t>RACE1</t>
   </si>
   <si>
-    <t>Y = Yes, box for race checked
+    <t>Y = Yes, box for race checked_x000D_
 N = No, box for race not checked</t>
   </si>
   <si>
@@ -1213,8 +1213,8 @@
     <t>RACE_MVR</t>
   </si>
   <si>
-    <t>R = Refused
-S = Sought, but Unknown
+    <t>R = Refused_x000D_
+S = Sought, but Unknown_x000D_
 C = Not Obtainable</t>
   </si>
   <si>
@@ -1281,8 +1281,8 @@
     <t>IDOB_YR</t>
   </si>
   <si>
-    <t>4 digit year = year of death or (year of death - 1)
-9999 = unknown
+    <t>4 digit year = year of death or (year of death - 1)_x000D_
+9999 = unknown_x000D_
 Blank</t>
   </si>
   <si>
@@ -1298,29 +1298,30 @@
     <t>BSTATE</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA
-YC = NEW YORK CITY
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA_x000D_
+YC = NEW YORK CITY_x000D_
+_x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -1909,7 +1910,7 @@
     <t>SPOUSELV</t>
   </si>
   <si>
-    <t>1=yes; 2=no; 8=unmarried; 9=unknown;
+    <t>1=yes; 2=no; 8=unmarried; 9=unknown;_x000D_
 blank if not reported</t>
   </si>
   <si>
@@ -2042,7 +2043,7 @@
     <t>RESSTATE</t>
   </si>
   <si>
-    <t>See codes used before new 2003 codes -
+    <t>See codes used before new 2003 codes -_x000D_
 Receiving state will recode</t>
   </si>
   <si>
@@ -2058,8 +2059,8 @@
     <t xml:space="preserve">DETHNICE </t>
   </si>
   <si>
-    <t>100 = NonHispanic
-200-299 = Hispanic
+    <t>100 = NonHispanic_x000D_
+200-299 = Hispanic_x000D_
 996-999 = Unknown</t>
   </si>
   <si>
@@ -2183,9 +2184,9 @@
     <t>TRANSPRT</t>
   </si>
   <si>
-    <t>DR=Driver/Operator
-PA=Passenger
-PE=Pedestrian
+    <t>DR=Driver/Operator_x000D_
+PA=Passenger_x000D_
+PE=Pedestrian_x000D_
 Enter full text if it does not fit above (blank for natural death)</t>
   </si>
   <si>
@@ -2213,7 +2214,7 @@
     <t>COUNTYCODE_I</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8; 999=unknown; 
+    <t>NCHS Instruction Manual: Part 8; 999=unknown; _x000D_
 Blank for natural death.</t>
   </si>
   <si>
@@ -2247,27 +2248,27 @@
     <t>STATECODE_I</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                 For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                 For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2499,27 +2500,27 @@
     <t>DISPSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                  For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                  For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2622,27 +2623,27 @@
     <t>FUNSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                       For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                       For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2775,27 +2776,27 @@
     <t>CERTSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                   For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                   For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2925,7 +2926,7 @@
     <t>MARITAL_DESCRIP</t>
   </si>
   <si>
-    <t>Free text for use of jurisdictions with domestic partnerships, other
+    <t>Free text for use of jurisdictions with domestic partnerships, other_x000D_
 types of relationships.</t>
   </si>
   <si>
@@ -3112,7 +3113,7 @@
     <t>gender</t>
   </si>
   <si>
-    <t>[AdministrativeGenderVS] - See [Note on Decedent Gender]</t>
+    <t>[AdministrativeGenderVS] - See [Note on Gender]</t>
   </si>
   <si>
     <t>MortalityRosterBundle</t>
@@ -3160,27 +3161,27 @@
     <t>BundleDocumentCodedCauseOfFetalDeath</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                        For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                        For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3196,26 +3197,26 @@
     <t>State, U.S. Territory or Canadian Province of Death - literal</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3279,28 +3280,28 @@
     <t>State, U.S. Territory or Canadian Province of Decedent's Residence - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3547,26 +3548,26 @@
     <t>STATE_T</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3579,7 +3580,7 @@
     <t>Void Flag</t>
   </si>
   <si>
-    <t>0 = default; valid record
+    <t>0 = default; valid record_x000D_
 1 = VOID record</t>
   </si>
   <si>
@@ -3637,10 +3638,10 @@
     <t>TPLACE</t>
   </si>
   <si>
-    <t>1 = Hospital
-2 = Clinic
-3 = Doctor's Office
-4 = Other
+    <t>1 = Hospital_x000D_
+2 = Clinic_x000D_
+3 = Doctor's Office_x000D_
+4 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -3668,7 +3669,7 @@
     <t>AGE</t>
   </si>
   <si>
-    <t>10-55
+    <t>10-55_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -3681,27 +3682,27 @@
     <t>State, U.S. Territory or Canadian Province of Residence (Patient) - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                     For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                     For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3771,12 +3772,12 @@
     <t>Patient's Marital Status</t>
   </si>
   <si>
-    <t>1 = Never Married
-2 = Now Married
-3 = Widowed
-4 = Divorced
-5 = Separated
-7 = Other (specify below)
+    <t>1 = Never Married_x000D_
+2 = Now Married_x000D_
+3 = Widowed_x000D_
+4 = Divorced_x000D_
+5 = Separated_x000D_
+7 = Other (specify below)_x000D_
 9 = Unknown or Not Stated</t>
   </si>
   <si>
@@ -3831,13 +3832,13 @@
     <t>ETHNIC_OLD</t>
   </si>
   <si>
-    <t>from single choice versus mark all
-0 = non-hispanic
-1 = Mexican
-2 = Puerto Rican
-3 = Cuban
-4 = Central of South American
-5 = Other or unknown hispanic
+    <t>from single choice versus mark all_x000D_
+0 = non-hispanic_x000D_
+1 = Mexican_x000D_
+2 = Puerto Rican_x000D_
+3 = Cuban_x000D_
+4 = Central of South American_x000D_
+5 = Other or unknown hispanic_x000D_
 9 = Not classifiable</t>
   </si>
   <si>
@@ -3847,15 +3848,15 @@
     <t>ETHNIC_OTH</t>
   </si>
   <si>
-    <t>Comma delimit multiple entries; 
+    <t>Comma delimit multiple entries; _x000D_
 Some states keep a version of multiple Hispanic origin that is not in the new format but something in between.</t>
   </si>
   <si>
     <t>Patient's Race--White</t>
   </si>
   <si>
-    <t>Y = Yes, box for race checked
-N = No, box for race not checked
+    <t>Y = Yes, box for race checked_x000D_
+N = No, box for race not checked_x000D_
 U = Unknown race (U in all race fields)</t>
   </si>
   <si>
@@ -3934,14 +3935,14 @@
     <t>RACE_OLD</t>
   </si>
   <si>
-    <t>From single choice versus mark all
-1 = white; 2 =  Black;
-3 = American Indian; 4 = Chinese
-5 = Japanese; 6 = Hawaiian;
-7 = Filipino; 8 = Other Asian/ Pac Islander;
-9 = not reported; A = Asian Indian; 
-B = Korean; C = Samoan;
-D = Vietnamese; E = Guamian;
+    <t>From single choice versus mark all_x000D_
+1 = white; 2 =  Black;_x000D_
+3 = American Indian; 4 = Chinese_x000D_
+5 = Japanese; 6 = Hawaiian;_x000D_
+7 = Filipino; 8 = Other Asian/ Pac Islander;_x000D_
+9 = not reported; A = Asian Indian; _x000D_
+B = Korean; C = Samoan;_x000D_
+D = Vietnamese; E = Guamian;_x000D_
 F = Multi-racial</t>
   </si>
   <si>
@@ -3951,7 +3952,7 @@
     <t>RACE_OTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma delimit multiple entries;
+    <t xml:space="preserve">Comma delimit multiple entries;_x000D_
 Some states keep a version of multiple race that is not in the new format but something in between. </t>
   </si>
   <si>
@@ -3961,7 +3962,7 @@
     <t>PREV_PREG</t>
   </si>
   <si>
-    <t>00-30
+    <t>00-30_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -3971,14 +3972,14 @@
     <t>PLBT</t>
   </si>
   <si>
-    <t>Previous live births,
+    <t>Previous live births,_x000D_
 Now living</t>
   </si>
   <si>
     <t>PLBL</t>
   </si>
   <si>
-    <t>Previous live births,
+    <t>Previous live births,_x000D_
 Now dead</t>
   </si>
   <si>
@@ -4009,7 +4010,7 @@
     <t>DLMP_MO</t>
   </si>
   <si>
-    <t>00-12
+    <t>00-12_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4019,7 +4020,7 @@
     <t>DLMP_DY</t>
   </si>
   <si>
-    <t>01-31 (based on month)
+    <t>01-31 (based on month)_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4029,7 +4030,7 @@
     <t>CWGEST</t>
   </si>
   <si>
-    <t>01-27
+    <t>01-27_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4099,18 +4100,18 @@
     <t>PROC_T</t>
   </si>
   <si>
-    <t>1 = Suction Curettage
-2 = Medical (Non-surgical; medication induced -- specify medication(s) in field below)
-3 = Dilation &amp; Evacuation (D&amp;E)
-4 = Intra-Uterine Instillation (Saline or Prostaglandin)
-5 = Vaginal Prostaglandin
-6 = Sharp Curettage (D&amp;C)
-7 = Hysterotomy/Hysterectomy
-8 = Other
+    <t>1 = Suction Curettage_x000D_
+2 = Medical (Non-surgical; medication induced -- specify medication(s) in field below)_x000D_
+3 = Dilation &amp; Evacuation (D&amp;E)_x000D_
+4 = Intra-Uterine Instillation (Saline or Prostaglandin)_x000D_
+5 = Vaginal Prostaglandin_x000D_
+6 = Sharp Curettage (D&amp;C)_x000D_
+7 = Hysterotomy/Hysterectomy_x000D_
+8 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Medical (non-surgical) procedure medication(s) literal 
+    <t xml:space="preserve">Medical (non-surgical) procedure medication(s) literal _x000D_
 </t>
   </si>
   <si>
@@ -4120,7 +4121,7 @@
     <t>Free form literal specifing medication(s) that terminated this pregnancy.</t>
   </si>
   <si>
-    <t xml:space="preserve">Termination other procedure literal 
+    <t xml:space="preserve">Termination other procedure literal _x000D_
 </t>
   </si>
   <si>
@@ -4136,15 +4137,15 @@
     <t>PROC-OTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeat up to 4 single digit codes                            
-0 = None                                                                                                                                                                                                                           1 = Suction Curettage
-2 = Medical (Non-surgical; medication induced)
-3 = Dilation &amp; Evacuation (D&amp;E)
-4 = Intra-Uterine Instillation (Saline or Prostaglandin)
-5 = Vaginal Prostaglandin
-6 = Sharp Curettage (D&amp;C)
-8 = Other
-9 = Unknown
+    <t xml:space="preserve">Repeat up to 4 single digit codes                            _x000D_
+0 = None                                                                                                                                                                                                                           1 = Suction Curettage_x000D_
+2 = Medical (Non-surgical; medication induced)_x000D_
+3 = Dilation &amp; Evacuation (D&amp;E)_x000D_
+4 = Intra-Uterine Instillation (Saline or Prostaglandin)_x000D_
+5 = Vaginal Prostaglandin_x000D_
+6 = Sharp Curettage (D&amp;C)_x000D_
+8 = Other_x000D_
+9 = Unknown_x000D_
 </t>
   </si>
   <si>
@@ -4154,7 +4155,7 @@
     <t>CALC_WGEST</t>
   </si>
   <si>
-    <t>00-95
+    <t>00-95_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4167,7 +4168,7 @@
     <t>Y, N, or U (if N or U, leave all other TP complications blank)</t>
   </si>
   <si>
-    <t>Hemorrhage
+    <t>Hemorrhage_x000D_
 (at time of procedure)</t>
   </si>
   <si>
@@ -4177,56 +4178,56 @@
     <t>Y, N, U (some jurisdictions may only collect hemorage data if above a certain volumn)</t>
   </si>
   <si>
-    <t>Infection
+    <t>Infection_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>INFECT_TP</t>
   </si>
   <si>
-    <t>Uterine perforation
+    <t>Uterine perforation_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>PERF_TP</t>
   </si>
   <si>
-    <t>Cervical laceration
+    <t>Cervical laceration_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>LACER_TP</t>
   </si>
   <si>
-    <t>Retained products
+    <t>Retained products_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>RETAN_TP</t>
   </si>
   <si>
-    <t>Death 
+    <t>Death _x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>DEATH_TP</t>
   </si>
   <si>
-    <t>Failure of first method 
+    <t>Failure of first method _x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>FAIL_TP</t>
   </si>
   <si>
-    <t>Other complications 
+    <t>Other complications _x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>OTHER_TP</t>
   </si>
   <si>
-    <t>Other complications literal 
+    <t>Other complications literal _x000D_
 (at time of procedure)</t>
   </si>
   <si>
@@ -4245,49 +4246,49 @@
     <t>Y, N, or U (if N or U, leave all other F1 complications blank)</t>
   </si>
   <si>
-    <t>Complications at followup
+    <t>Complications at followup_x000D_
 at same facility</t>
   </si>
   <si>
     <t>COMP_F1</t>
   </si>
   <si>
-    <t>Hemorrhage
+    <t>Hemorrhage_x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>HEMOR_F1</t>
   </si>
   <si>
-    <t>Infection 
+    <t>Infection _x000D_
 (at time of  follow up at this facility)</t>
   </si>
   <si>
     <t>INFECT_F1</t>
   </si>
   <si>
-    <t>Uterine perforation 
+    <t>Uterine perforation _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>PERF_F1</t>
   </si>
   <si>
-    <t>Cervical laceration 
+    <t>Cervical laceration _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>LACER_F1</t>
   </si>
   <si>
-    <t>Retained products 
+    <t>Retained products _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>RETAN_F1</t>
   </si>
   <si>
-    <t>Death 
+    <t>Death _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
@@ -4306,7 +4307,7 @@
     <t>OTHER_F1</t>
   </si>
   <si>
-    <t>Other complications literal 
+    <t>Other complications literal _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
@@ -4325,70 +4326,70 @@
     <t>Y, N, or U (if N or U, leave all other F2 complications blank)</t>
   </si>
   <si>
-    <t>Complications 
+    <t>Complications _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>COMP_F2</t>
   </si>
   <si>
-    <t>Hemorrhage
+    <t>Hemorrhage_x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>HEMOR_F2</t>
   </si>
   <si>
-    <t>Infection 
+    <t>Infection _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>INFECT_F2</t>
   </si>
   <si>
-    <t>Uterine perforation  
+    <t>Uterine perforation  _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>PERF_F2</t>
   </si>
   <si>
-    <t>Cervical laceration  
+    <t>Cervical laceration  _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>LACER_F2</t>
   </si>
   <si>
-    <t>Retained products 
+    <t>Retained products _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>RETAN_F2</t>
   </si>
   <si>
-    <t>Death 
+    <t>Death _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>DEATH_F2</t>
   </si>
   <si>
-    <t>Failure of first method 
+    <t>Failure of first method _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>FAIL_F2</t>
   </si>
   <si>
-    <t xml:space="preserve">Other complications 
+    <t xml:space="preserve">Other complications _x000D_
 (at time of followup at other facility) </t>
   </si>
   <si>
     <t>OTHER_F2</t>
   </si>
   <si>
-    <t>Other complications literal 
+    <t>Other complications literal _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
@@ -4398,17 +4399,17 @@
     <t>Free form literal of specified other complication at time of followup at other facility.</t>
   </si>
   <si>
-    <t>Site of follow-up visit 
+    <t>Site of follow-up visit _x000D_
 (at other facility)</t>
   </si>
   <si>
     <t>SITE_F2</t>
   </si>
   <si>
-    <t>1 = physician's office
-2 = clinic
-3 = hospital
-4 = other, specify
+    <t>1 = physician's office_x000D_
+2 = clinic_x000D_
+3 = hospital_x000D_
+4 = other, specify_x000D_
 9 = unknown</t>
   </si>
   <si>
@@ -4688,8 +4689,8 @@
     <t>FSEX</t>
   </si>
   <si>
-    <t xml:space="preserve">M = Male
-F = Female
+    <t xml:space="preserve">M = Male_x000D_
+F = Female_x000D_
 U = Unknown </t>
   </si>
   <si>
@@ -4726,13 +4727,13 @@
     <t>Place Where Delivery Occurred</t>
   </si>
   <si>
-    <t>1 = Hospital
-2 = Freestanding Birth Center
-3 = Home (Intended)
-4 = Home (Not Intended)
-5 = Home (Unknown if Intended)
-6 = Clinic/Doctor's Office
-7 = Other
+    <t>1 = Hospital_x000D_
+2 = Freestanding Birth Center_x000D_
+3 = Home (Intended)_x000D_
+4 = Home (Not Intended)_x000D_
+5 = Home (Unknown if Intended)_x000D_
+6 = Clinic/Doctor's Office_x000D_
+7 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -4790,7 +4791,7 @@
     <t>MAGE_BYPASS</t>
   </si>
   <si>
-    <t xml:space="preserve">0 = Edit Passed
+    <t xml:space="preserve">0 = Edit Passed_x000D_
 1 = Data Queried </t>
   </si>
   <si>
@@ -4809,27 +4810,27 @@
     <t>BPLACEC_ST_TER</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -4854,27 +4855,27 @@
     <t>State, U.S. Territory or Canadian Province of Residence (Mother) - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -4884,8 +4885,8 @@
     <t>Residence of Mother--Inside City/Town Limits</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -4952,8 +4953,8 @@
     <t>MEDUC_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Data Queried and Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Data Queried and Verified_x000D_
 2 = Edit Failed, Data Queried, but not Verified</t>
   </si>
   <si>
@@ -5374,11 +5375,11 @@
     <t>ATTEND</t>
   </si>
   <si>
-    <t>1 = MD
-2 = DO
-3 = CNM/CM
-4 = Other midwife
-5 = Other (specify)
+    <t>1 = MD_x000D_
+2 = DO_x000D_
+3 = CNM/CM_x000D_
+4 = Other midwife_x000D_
+5 = Other (specify)_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -5430,7 +5431,7 @@
     <t>DOFP_YR</t>
   </si>
   <si>
-    <t>4 digit year; year of delivery or
+    <t>4 digit year; year of delivery or_x000D_
 (year of delivery - 1), 8888, 9999</t>
   </si>
   <si>
@@ -5467,8 +5468,8 @@
     <t>NPREV_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Number Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Number Verified_x000D_
 2 = Edit Failed, Number not Verified</t>
   </si>
   <si>
@@ -5502,8 +5503,8 @@
     <t>HGT_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Number Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Number Verified_x000D_
 2 = Edit Failed, Number not  Verified</t>
   </si>
   <si>
@@ -5531,8 +5532,8 @@
     <t>PWGT_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Verified_x000D_
 2 = Edit Failed, not Verified</t>
   </si>
   <si>
@@ -5599,8 +5600,8 @@
     <t>YLLB</t>
   </si>
   <si>
-    <t>4 digit year;
-(year of mother's birth + 10) through
+    <t>4 digit year;_x000D_
+(year of mother's birth + 10) through_x000D_
 year of delivery, 8888, 9999</t>
   </si>
   <si>
@@ -5658,8 +5659,8 @@
     <t>Date Last Normal Menses Began--Year</t>
   </si>
   <si>
-    <t>4 digit year; year of delivery or
-(year of delivery - 1) or
+    <t>4 digit year; year of delivery or_x000D_
+(year of delivery - 1) or_x000D_
 (year of delivery - 2), 9999</t>
   </si>
   <si>
@@ -5684,9 +5685,9 @@
     <t>See [note on missing pregnancy risk factors data]</t>
   </si>
   <si>
-    <t>Update risk factors (old Observation-pregnancy-risk-factor)
-STU 1 listed:
-IJE Natality Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART
+    <t>Update risk factors (old Observation-pregnancy-risk-factor)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART_x000D_
 IJE Fetal Death Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART</t>
   </si>
   <si>
@@ -5777,7 +5778,7 @@
     <t>NPCES_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
+    <t>0 = Edit Passed_x000D_
 1 = Edit Failed, Verified</t>
   </si>
   <si>
@@ -5865,9 +5866,9 @@
     <t>PRES</t>
   </si>
   <si>
-    <t>1 = Cephalic
-2 = Breech
-3 = Other
+    <t>1 = Cephalic_x000D_
+2 = Breech_x000D_
+3 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -5883,10 +5884,10 @@
     <t>ROUT</t>
   </si>
   <si>
-    <t>1 = Spontaneous
-2 = Forceps
-3 = Vacuum
-4 = Cesarean
+    <t>1 = Spontaneous_x000D_
+2 = Forceps_x000D_
+3 = Vacuum_x000D_
+4 = Cesarean_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -5905,9 +5906,9 @@
     <t>TLAB</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
-U = Unknown
+    <t>Y = Yes_x000D_
+N = No_x000D_
+U = Unknown_x000D_
 X = Not Applicable</t>
   </si>
   <si>
@@ -5926,9 +5927,9 @@
     <t>MTR</t>
   </si>
   <si>
-    <t>Update maternal morbidity (old Condition-maternal-morbidity)
-STU 1 listed:
-IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT
+    <t>Update maternal morbidity (old Condition-maternal-morbidity)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT_x000D_
 IJE Fetal Death Data Elements: RUT, AINT</t>
   </si>
   <si>
@@ -5977,10 +5978,10 @@
     <t>UOPR</t>
   </si>
   <si>
-    <t>Update maternal morbidity (old Condition-maternal-morbidity)
-STU 1 listed:
-IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT
-IJE Fetal Death Data Elements: RUT, AINT
+    <t>Update maternal morbidity (old Condition-maternal-morbidity)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT_x000D_
+IJE Fetal Death Data Elements: RUT, AINT_x000D_
 (new) UOPR</t>
   </si>
   <si>
@@ -5999,8 +6000,8 @@
     <t>FW_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
-1 = Queried data correct, out of range
+    <t>0 = Off_x000D_
+1 = Queried data correct, out of range_x000D_
 2 = Queried, failed  delivery weight/gestation edit</t>
   </si>
   <si>
@@ -6025,7 +6026,7 @@
     <t>OWGEST_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
+    <t>0 = Off_x000D_
 1 = Queried data correct, out of range</t>
   </si>
   <si>
@@ -6038,9 +6039,9 @@
     <t>ETIME</t>
   </si>
   <si>
-    <t>N = At assessment, no labor
-L = At assessment, labor
-A = Labor, no assessment
+    <t>N = At assessment, no labor_x000D_
+L = At assessment, labor_x000D_
+A = Labor, no assessment_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -6053,8 +6054,8 @@
     <t>Was an Autopsy Performed?</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 P = Planned</t>
   </si>
   <si>
@@ -6076,8 +6077,8 @@
     <t>Were Autopsy or Histological Placental Examination Results Used in Determining the Cause of Fetal Death?</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 X = Not Applicable</t>
   </si>
   <si>
@@ -6126,8 +6127,8 @@
     <t>PLUR_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
-1 = Queried, and Correct
+    <t>0 = Off_x000D_
+1 = Queried, and Correct_x000D_
 2 = Plurality/Set Order Queried, Inconsistent</t>
   </si>
   <si>
@@ -6197,9 +6198,9 @@
     <t>DOWT</t>
   </si>
   <si>
-    <t>C = Confirmed
-P = Pending
-N = No
+    <t>C = Confirmed_x000D_
+P = Pending_x000D_
+N = No_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -6221,10 +6222,10 @@
     <t>&gt;=year of delivery</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Code structure description differs here
-Code sent back to state VRO
-For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Code structure description differs here_x000D_
+Code sent back to state VRO_x000D_
+For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -6240,10 +6241,10 @@
     <t>NCHS USE ONLY: Receipt date -- Day</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Code structure description differs here
-Code sent back to state VRO
-Note: Marked as NCHS USE ONLY, but VRDR does address this. For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Code structure description differs here_x000D_
+Code sent back to state VRO_x000D_
+Note: Marked as NCHS USE ONLY, but VRDR does address this. For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -6286,9 +6287,9 @@
     <t>INFT_DRG</t>
   </si>
   <si>
-    <t>Y = Yes (BLANK IF NOT ADDED)
-N = No
-X = Not Applicable
+    <t>Y = Yes (BLANK IF NOT ADDED)_x000D_
+N = No_x000D_
+X = Not Applicable_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -6325,7 +6326,7 @@
     <t>COD18a1</t>
   </si>
   <si>
-    <t>Y = Yes
+    <t>Y = Yes_x000D_
 N = No</t>
   </si>
   <si>
@@ -7013,9 +7014,9 @@
     <t>string(25)</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-NCHS does not use
-BFDR defines "ObservationPresentJob" profile. 
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+NCHS does not use_x000D_
+BFDR defines "ObservationPresentJob" profile. _x000D_
 BFDR and VRDR use different profiles</t>
   </si>
   <si>
@@ -7577,24 +7578,24 @@
     <t>MRACEBG_C</t>
   </si>
   <si>
-    <t>01 = White
-02 = Black
-03 = American Indian/Alaskan Native
-04 = Asian Indian
-05 = Chinese
-06 = Filipino
-07 = Japanese
-08 = Korean
-09 = Vietnamese
-10 = Other Asian
-11 = Native Hawaiian
-12 = Guamanian
-13 = Samoan
-14 = Other Pacific Islander
-15 = Other
-21 = Bridged White
-22 = Bridged Black
-23 = Bridged American Indian/Alaskan Native
+    <t>01 = White_x000D_
+02 = Black_x000D_
+03 = American Indian/Alaskan Native_x000D_
+04 = Asian Indian_x000D_
+05 = Chinese_x000D_
+06 = Filipino_x000D_
+07 = Japanese_x000D_
+08 = Korean_x000D_
+09 = Vietnamese_x000D_
+10 = Other Asian_x000D_
+11 = Native Hawaiian_x000D_
+12 = Guamanian_x000D_
+13 = Samoan_x000D_
+14 = Other Pacific Islander_x000D_
+15 = Other_x000D_
+21 = Bridged White_x000D_
+22 = Bridged Black_x000D_
+23 = Bridged American Indian/Alaskan Native_x000D_
 24 = Bridged Asian &amp; Pacific Islander</t>
   </si>
   <si>
@@ -7715,24 +7716,24 @@
     <t>Informant's Relationship to Fetus</t>
   </si>
   <si>
-    <t>1 = Mother
-2 = Father
-3 = Sibling
-4 = Other relative
-5 = Other
+    <t>1 = Mother_x000D_
+2 = Father_x000D_
+3 = Sibling_x000D_
+4 = Other relative_x000D_
+5 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Only similar item is Mortality: "Informant's Relationship (INFORMRELATE), which uses VRDR Decedent  contact.type.text   string (30 characters)
-VRCPL has:
-  - Patient-decedent-fetus, 
-  - Related Person - Parent Vital Records   
-  - RelatedPerson - Father Natural Vital Records         
-  - RelatedPerson - Father Vital Records         
-  - RelatedPerson - Mother Gestational Vital Records         
-  - RelatedPerson - Mother Vital Records
-NOTE that the IJE Code Structure Description here includes Sibling and others
-Saul notes: VRDR uses fields that can be from a controlled vocabulary or any arbitrary string (e.g., CERTL in  http://build.fhir.org/ig/HL7/vrdr/branches/master/StructureDefinition-vrdr-death-certification.html) with a consistent pattern (I think
+    <t xml:space="preserve">Only similar item is Mortality: "Informant's Relationship (INFORMRELATE), which uses VRDR Decedent  contact.type.text   string (30 characters)_x000D_
+VRCPL has:_x000D_
+  - Patient-decedent-fetus, _x000D_
+  - Related Person - Parent Vital Records   _x000D_
+  - RelatedPerson - Father Natural Vital Records         _x000D_
+  - RelatedPerson - Father Vital Records         _x000D_
+  - RelatedPerson - Mother Gestational Vital Records         _x000D_
+  - RelatedPerson - Mother Vital Records_x000D_
+NOTE that the IJE Code Structure Description here includes Sibling and others_x000D_
+Saul notes: VRDR uses fields that can be from a controlled vocabulary or any arbitrary string (e.g., CERTL in  http://build.fhir.org/ig/HL7/vrdr/branches/master/StructureDefinition-vrdr-death-certification.html) with a consistent pattern (I think_x000D_
 there are two such fields). </t>
   </si>
   <si>
@@ -7787,9 +7788,9 @@
     <t>Deprecated, see [VRFM]</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Mortality (VRDR) uses   DeathCertificate  extension[replaceStatus].valuecodeable   [ReplaceStatusVS]
-VRDR addresses in the VRDR Messaging IG. 
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Mortality (VRDR) uses   DeathCertificate  extension[replaceStatus].valuecodeable   [ReplaceStatusVS]_x000D_
+VRDR addresses in the VRDR Messaging IG. _x000D_
 Decision: Births should behave the same as deaths.</t>
   </si>
   <si>
@@ -7805,30 +7806,31 @@
     <t>State, U.S. Territory or Canadian Province of Birth (Infant) - code</t>
   </si>
   <si>
-    <t xml:space="preserve">
-NCHS Instruction Manual: Part 8
-ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA
-YC = NEW YORK CITY
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>_x000D_
+NCHS Instruction Manual: Part 8_x000D_
+ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA_x000D_
+YC = NEW YORK CITY_x000D_
+_x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -7844,12 +7846,12 @@
     <t>identifier.extension[localFileNumber2].value</t>
   </si>
   <si>
-    <t>male = Male
-female = Female
+    <t>male = Male_x000D_
+female = Female_x000D_
 other = Other unknown = Unknown</t>
   </si>
   <si>
-    <t>[USCorePatient] requires gender - can be 'unknown'. genderIdentity field is not required.</t>
+    <t xml:space="preserve">[USCorePatient] requires gender - can be 'unknown'. See [Note on Gender] </t>
   </si>
   <si>
     <t>Time of Birth</t>
@@ -7861,8 +7863,8 @@
     <t>ISEX</t>
   </si>
   <si>
-    <t>M = Male
-F = Female
+    <t>M = Male_x000D_
+F = Female_x000D_
 N = Not Yet Determined</t>
   </si>
   <si>
@@ -7896,31 +7898,31 @@
     <t>4 digit year (&lt; year of birth of child);  9999 = unknown</t>
   </si>
   <si>
-    <t>0 = Edit Passed
+    <t>0 = Edit Passed_x000D_
 1 = Data Queried</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -7930,27 +7932,27 @@
     <t>Residence of Mother--City</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA        For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA        For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -7990,8 +7992,8 @@
     <t>Literal; blank</t>
   </si>
   <si>
-    <t xml:space="preserve">NCHS Appendix E
-(values for fields 62 - 77 returned from NCHS)
+    <t xml:space="preserve">NCHS Appendix E_x000D_
+(values for fields 62 - 77 returned from NCHS)_x000D_
 </t>
   </si>
   <si>
@@ -8001,7 +8003,7 @@
     <t>component[ThirdEditedCode].value, &lt;br /&gt;code=CodeSystemLocalObservationsCodesVitalRecords#codedraceandethnicityMother</t>
   </si>
   <si>
-    <t>NCHS Appendix E
+    <t>NCHS Appendix E_x000D_
 (values for fields 108 - 123 returned from NCHS)</t>
   </si>
   <si>
@@ -8023,11 +8025,11 @@
     <t>01-31 (based on month), 88=no care, 99=unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">4 digit year; year of child's birth or
+    <t xml:space="preserve">4 digit year; year of child's birth or_x000D_
 (year of child's birth - 1), 8888=no care, 9999=unknown </t>
   </si>
   <si>
-    <t>4 digit year; year of child's birth or 
+    <t>4 digit year; year of child's birth or _x000D_
 (year of child's birth - 1), 8888=no care, 9999=unknown</t>
   </si>
   <si>
@@ -8058,7 +8060,7 @@
     <t>ObservationNumberOtherPregnancyOutcomes</t>
   </si>
   <si>
-    <t>4 digit year;(year of mother's birth + 10) through
+    <t>4 digit year;(year of mother's birth + 10) through_x000D_
 year of child's birth, 8888, 9999</t>
   </si>
   <si>
@@ -8080,13 +8082,13 @@
     <t>PAY</t>
   </si>
   <si>
-    <t>1 = Medicaid
-2 = Private Insurance
-3 = Self-pay
-4 = Indian Health Service
-5 = CHAMPUS/TRICARE
-6 = Other Government (Fed, State, Local) 
-8 = Other
+    <t>1 = Medicaid_x000D_
+2 = Private Insurance_x000D_
+3 = Self-pay_x000D_
+4 = Indian Health Service_x000D_
+5 = CHAMPUS/TRICARE_x000D_
+6 = Other Government (Fed, State, Local) _x000D_
+8 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -8099,8 +8101,8 @@
     <t>[BirthAndFetalDeathFinancialClassVS] </t>
   </si>
   <si>
-    <t>4 digit year; year of child's birth 
-or (year of child's birth - 1)
+    <t>4 digit year; year of child's birth _x000D_
+or (year of child's birth - 1)_x000D_
 or (year of child's birth - 2), 9999</t>
   </si>
   <si>
@@ -8233,8 +8235,8 @@
     <t>See [note on missing characteristics of labor and delivery data]</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
-STU 1 listed:
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
+STU 1 listed:_x000D_
 IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN</t>
   </si>
   <si>
@@ -8289,9 +8291,9 @@
     <t>MECS</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
-STU 1 listed:
-IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN_x000D_
 (new) MECS</t>
   </si>
   <si>
@@ -8301,9 +8303,9 @@
     <t>FINT</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
-STU 1 listed:
-IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN_x000D_
 (new) FINT</t>
   </si>
   <si>
@@ -8349,8 +8351,8 @@
     <t>BW_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
-1 = Queried data correct, out of range
+    <t>0 = Off_x000D_
+1 = Queried data correct, out of range_x000D_
 2 = Queried, failed birthweight/gestation edit</t>
   </si>
   <si>
@@ -8390,8 +8392,8 @@
     <t>ObservationNumberLiveBirthsThisDelivery</t>
   </si>
   <si>
-    <t>0 = OFF
-1 = Queried, and Correct
+    <t>0 = OFF_x000D_
+1 = Queried, and Correct_x000D_
 2 = Plurality/Set Order Queried, Inconsistent</t>
   </si>
   <si>
@@ -8407,8 +8409,8 @@
     <t>See [note on missing abnormal conditions of newborn data]</t>
   </si>
   <si>
-    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)
-STU 1 listed:
+    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)_x000D_
+STU 1 listed:_x000D_
 IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH</t>
   </si>
   <si>
@@ -8466,9 +8468,9 @@
     <t>BINJ</t>
   </si>
   <si>
-    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)
-STU 1 listed:
-IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH
+    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH_x000D_
 (new) BINJ</t>
   </si>
   <si>
@@ -8568,8 +8570,8 @@
     <t>ILIV</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 U = Infant transferred, Status Unknown</t>
   </si>
   <si>
@@ -8588,9 +8590,9 @@
     <t>leave blank</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Code sent back to state VRO
-For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Code sent back to state VRO_x000D_
+For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -8600,10 +8602,10 @@
     <t>Risk Factors--Infertility: Fertility Enhancing Drugs  (RECOMMENDED ADDITION EFFECTIVE 2004)</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
-X = Not Applicable
-U = Unknown
+    <t>Y = Yes_x000D_
+N = No_x000D_
+X = Not Applicable_x000D_
+U = Unknown_x000D_
 (BLANK IF NOT ADDED)</t>
   </si>
   <si>
@@ -8760,27 +8762,27 @@
     <t>Refer to NCHS Instruction Manual Part 19, Industry and Occupation Coding for Death Certificates, 2003. Leave blank if using a coding system other than this</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -8904,8 +8906,8 @@
     <t>SSN_MULT_BTH_CD</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 or blank</t>
   </si>
   <si>
@@ -8954,12 +8956,12 @@
     <t>CERTIF</t>
   </si>
   <si>
-    <t>1 = MD
-2 = DO
-3 = CNM/CM
-4 = Other midwife
-5 = Other (specify) 
-6 = Hospital Admin
+    <t>1 = MD_x000D_
+2 = DO_x000D_
+3 = CNM/CM_x000D_
+4 = Other midwife_x000D_
+5 = Other (specify) _x000D_
+6 = Hospital Admin_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -9008,51 +9010,51 @@
     <t>Deprecated,  see [VRFM]</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA              For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA              For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA            For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA            For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -9128,7 +9130,7 @@
     <t>Residence Street number</t>
   </si>
   <si>
-    <t>For use of jurisdictions with domestic partnerships, other
+    <t>For use of jurisdictions with domestic partnerships, other_x000D_
 types of relationships.</t>
   </si>
   <si>
@@ -9153,26 +9155,26 @@
     <t>Death Jurisdiction - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual Part 8A
- For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
- For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual Part 8A_x000D_
+ For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+ For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -9639,7 +9641,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:R277"/>
+  <dimension ref="A1:S277"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9656,7 +9658,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -9711,8 +9713,9 @@
       <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9755,7 +9758,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9798,7 +9801,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>6</v>
       </c>
@@ -9841,7 +9844,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>6</v>
       </c>
@@ -9881,7 +9884,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>7</v>
       </c>
@@ -9924,7 +9927,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>8</v>
       </c>
@@ -9967,7 +9970,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>9</v>
       </c>
@@ -10010,7 +10013,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>9</v>
       </c>
@@ -10049,7 +10052,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>10</v>
       </c>
@@ -10092,7 +10095,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>11</v>
       </c>
@@ -10135,7 +10138,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>12</v>
       </c>
@@ -10178,7 +10181,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>13</v>
       </c>
@@ -10221,7 +10224,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10264,7 +10267,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10305,7 +10308,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>15</v>
       </c>
@@ -21118,7 +21121,7 @@
   <sheetPr>
     <tabColor rgb="FFFF99CC"/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21135,7 +21138,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -21190,8 +21193,9 @@
       <c r="R1" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="B2">
         <v>1</v>
       </c>
@@ -21228,7 +21232,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -21263,7 +21267,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -21298,7 +21302,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -21333,7 +21337,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -21370,7 +21374,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="B7" t="s">
         <v>946</v>
       </c>
@@ -21407,7 +21411,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -21444,7 +21448,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -21481,7 +21485,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -21518,7 +21522,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -21555,7 +21559,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -21592,7 +21596,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>431</v>
       </c>
@@ -21632,7 +21636,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>432</v>
       </c>
@@ -21672,7 +21676,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>433</v>
       </c>
@@ -21712,7 +21716,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>434</v>
       </c>
@@ -22970,7 +22974,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:R160"/>
+  <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -22987,7 +22991,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -23042,8 +23046,9 @@
       <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>272</v>
       </c>
@@ -23086,7 +23091,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>430</v>
       </c>
@@ -23126,7 +23131,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>273</v>
       </c>
@@ -23169,7 +23174,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>275</v>
       </c>
@@ -23212,7 +23217,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>276</v>
       </c>
@@ -23255,7 +23260,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>277</v>
       </c>
@@ -23296,7 +23301,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>278</v>
       </c>
@@ -23337,7 +23342,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>279</v>
       </c>
@@ -23380,7 +23385,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>280</v>
       </c>
@@ -23421,7 +23426,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>281</v>
       </c>
@@ -23462,7 +23467,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>282</v>
       </c>
@@ -23505,7 +23510,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>283</v>
       </c>
@@ -23548,7 +23553,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>284</v>
       </c>
@@ -23591,7 +23596,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>285</v>
       </c>
@@ -23634,7 +23639,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>286</v>
       </c>
@@ -29767,7 +29772,7 @@
   <sheetPr>
     <tabColor rgb="FFCC99FF"/>
   </sheetPr>
-  <dimension ref="A1:R160"/>
+  <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -29784,7 +29789,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -29839,8 +29844,9 @@
       <c r="R1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1183</v>
       </c>
@@ -29873,7 +29879,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1184</v>
       </c>
@@ -29906,7 +29912,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1185</v>
       </c>
@@ -29939,7 +29945,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1186</v>
       </c>
@@ -29972,7 +29978,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1187</v>
       </c>
@@ -30005,7 +30011,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1188</v>
       </c>
@@ -30038,7 +30044,7 @@
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1189</v>
       </c>
@@ -30071,7 +30077,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1190</v>
       </c>
@@ -30104,7 +30110,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1191</v>
       </c>
@@ -30137,7 +30143,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>1192</v>
       </c>
@@ -30170,7 +30176,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1193</v>
       </c>
@@ -30203,7 +30209,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>1194</v>
       </c>
@@ -30236,7 +30242,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>1195</v>
       </c>
@@ -30269,7 +30275,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>1196</v>
       </c>
@@ -30302,7 +30308,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>1197</v>
       </c>
@@ -35098,7 +35104,7 @@
   <sheetPr>
     <tabColor rgb="FFFFCC99"/>
   </sheetPr>
-  <dimension ref="A1:R370"/>
+  <dimension ref="A1:S370"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -35115,7 +35121,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -35170,8 +35176,9 @@
       <c r="R1" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>818</v>
       </c>
@@ -35213,7 +35220,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>819</v>
       </c>
@@ -35255,7 +35262,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>820</v>
       </c>
@@ -35294,7 +35301,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>820</v>
       </c>
@@ -35333,7 +35340,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>820</v>
       </c>
@@ -35372,7 +35379,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>821</v>
       </c>
@@ -35410,7 +35417,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>822</v>
       </c>
@@ -35449,7 +35456,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>822</v>
       </c>
@@ -35488,7 +35495,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>822</v>
       </c>
@@ -35527,7 +35534,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>823</v>
       </c>
@@ -35569,7 +35576,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>824</v>
       </c>
@@ -35611,7 +35618,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>825</v>
       </c>
@@ -35653,7 +35660,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>826</v>
       </c>
@@ -35695,7 +35702,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>827</v>
       </c>
@@ -35737,7 +35744,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>828</v>
       </c>
@@ -49870,7 +49877,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFFF"/>
   </sheetPr>
-  <dimension ref="A1:R368"/>
+  <dimension ref="A1:S368"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -49887,7 +49894,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -49942,8 +49949,9 @@
       <c r="R1" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="8"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>465</v>
       </c>
@@ -49985,7 +49993,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>466</v>
       </c>
@@ -50027,7 +50035,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>467</v>
       </c>
@@ -50066,7 +50074,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>467</v>
       </c>
@@ -50105,7 +50113,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>467</v>
       </c>
@@ -50144,7 +50152,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>468</v>
       </c>
@@ -50182,7 +50190,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>469</v>
       </c>
@@ -50221,7 +50229,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>469</v>
       </c>
@@ -50260,7 +50268,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>469</v>
       </c>
@@ -50299,7 +50307,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -50338,7 +50346,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -50377,7 +50385,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -50416,7 +50424,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -50455,7 +50463,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -50494,7 +50502,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -64822,7 +64830,7 @@
   <sheetPr>
     <tabColor rgb="FFC4BD97"/>
   </sheetPr>
-  <dimension ref="A1:R350"/>
+  <dimension ref="A1:S350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -64839,7 +64847,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -64894,8 +64902,9 @@
       <c r="R1" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1342</v>
       </c>
@@ -64922,7 +64931,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1343</v>
       </c>
@@ -64949,7 +64958,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1344</v>
       </c>
@@ -64976,7 +64985,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1345</v>
       </c>
@@ -65003,7 +65012,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1346</v>
       </c>
@@ -65030,7 +65039,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1347</v>
       </c>
@@ -65057,7 +65066,7 @@
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1348</v>
       </c>
@@ -65084,7 +65093,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1349</v>
       </c>
@@ -65111,7 +65120,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1350</v>
       </c>
@@ -65138,7 +65147,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>1351</v>
       </c>
@@ -65165,7 +65174,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1352</v>
       </c>
@@ -65192,7 +65201,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>1353</v>
       </c>
@@ -65217,7 +65226,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>1354</v>
       </c>
@@ -65242,7 +65251,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>1355</v>
       </c>
@@ -65269,7 +65278,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>1356</v>
       </c>

</xml_diff>